<commit_message>
[UPDATE] Excel de ISBNs en el proceso de lectura
</commit_message>
<xml_diff>
--- a/Practica1/ProcesoLectura/Data/ISBNS.xlsx
+++ b/Practica1/ProcesoLectura/Data/ISBNS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3a4c74272cedf01d/Escritorio/Universidad/Practicas Finales/Inteligencia Artificial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{75F9DA85-6412-421E-AD36-DA4F03FCEEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E264361-89B9-40AF-B674-A515C1A7ABC2}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{75F9DA85-6412-421E-AD36-DA4F03FCEEFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A305FE4D-36B4-44DE-842F-A658312DB081}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF211DC2-FC04-41AC-9102-3344C0DE50AC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{FF211DC2-FC04-41AC-9102-3344C0DE50AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>ISBN</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>978-5566778899</t>
+  </si>
+  <si>
+    <t>9780307455376</t>
+  </si>
+  <si>
+    <t>979-1-876543-21-0</t>
+  </si>
+  <si>
+    <t>9788423687268</t>
   </si>
 </sst>
 </file>
@@ -146,8 +155,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,15 +496,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA65EA80-D8A2-44B8-97ED-35175390AF26}">
-  <dimension ref="A1:A25"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D8" activeCellId="1" sqref="C25 D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -544,81 +554,101 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
+      <c r="A12" s="1">
+        <v>5556667778</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>13</v>
+      <c r="A17" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>